<commit_message>
Added AboutContactPage.java and AboutContactPageTest.java
</commit_message>
<xml_diff>
--- a/Hubspot/src/main/java/com/qa/hubspot/testdata/TestData.xlsx
+++ b/Hubspot/src/main/java/com/qa/hubspot/testdata/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="14295" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14835" windowHeight="6420"/>
   </bookViews>
   <sheets>
     <sheet name="contacts" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A1:L20"/>
 </workbook>
 </file>
 
@@ -450,7 +451,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -492,82 +493,85 @@
         <v>7</v>
       </c>
     </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="1" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1"/>
-    <hyperlink ref="A4" r:id="rId2"/>
-    <hyperlink ref="A5" r:id="rId3"/>
-    <hyperlink ref="A6" r:id="rId4"/>
+    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>